<commit_message>
Reto 2 - 65% (Grafcas errores)
</commit_message>
<xml_diff>
--- a/Retos/Reto 3/Sucesion_Errores.xlsx
+++ b/Retos/Reto 3/Sucesion_Errores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="19560" windowHeight="7635" activeTab="2"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="19560" windowHeight="7635" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" r:id="rId1"/>
@@ -4972,7 +4972,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -16959,7 +16958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>

</xml_diff>